<commit_message>
Fix errors in javadoc
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/FrancisQRTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/FrancisQRTest.xlsx
@@ -470,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T27" sqref="T27:W31"/>
     </sheetView>
   </sheetViews>
@@ -5548,723 +5548,723 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*2-0.7</f>
-        <v>-0.56444175895355686</v>
+        <v>0.53173262986914116</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:I16" ca="1" si="0">RAND()*2-0.7</f>
-        <v>-0.20644039297691785</v>
+        <v>0.52713967737936018</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98913425857932369</v>
+        <v>1.2815262107669363</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2430076318927517</v>
+        <v>8.5421740343009978E-2</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.42041573515330755</v>
+        <v>0.28414257841892909</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77470631463473971</v>
+        <v>0.35506907750559114</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.57857709156611792</v>
+        <v>0.2842867401368887</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8985248300749924</v>
+        <v>-4.0317403277452257E-3</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87880695017026955</v>
+        <v>-0.62957678814169782</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:I19" ca="1" si="1">RAND()*2-0.7</f>
-        <v>-0.15977262026151107</v>
+        <v>-0.16484108846613887</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85810416838408377</v>
+        <v>0.63656257816085682</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93313037185130243</v>
+        <v>0.71818448159165094</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72261346771813573</v>
+        <v>0.64897847446035017</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.52561991972901967</v>
+        <v>-0.49818996707679619</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50243020753835532</v>
+        <v>1.137663950322731</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.17252906036080851</v>
+        <v>1.2360479644033069</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31371715109847376</v>
+        <v>-2.1322541294110042E-2</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77116115424851084</v>
+        <v>0.93448543260781491</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47043360565626258</v>
+        <v>0.84437746593352059</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72796730401817378</v>
+        <v>1.0411496925089103</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26033997343317261</v>
+        <v>0.40941254206924449</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.31769509555825937</v>
+        <v>-0.33367757803879705</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84553725113301148</v>
+        <v>0.96142956096985066</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2068288877299207</v>
+        <v>1.0783561874859449</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0739516628089774</v>
+        <v>0.28818260492749737</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53948149058087025</v>
+        <v>0.13615210616965467</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.48333521763871334</v>
+        <v>-0.65258974852054408</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78816813015612208</v>
+        <v>0.7042807182308839</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.54265382883554958</v>
+        <v>0.56081637770016735</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19994225059124626</v>
+        <v>0.68840215152133033</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.284462763689006</v>
+        <v>0.34238174523710319</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3137502521437463</v>
+        <v>1.1720253978006898</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.50386277654410061</v>
+        <v>0.62890041057198998</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0030539413932775</v>
+        <v>0.39558582552919086</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16018006955560571</v>
+        <v>1.1740073361884584</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.4428264442136109E-2</v>
+        <v>0.808644027124793</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42441705589113332</v>
+        <v>0.99565700091201936</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4270901770474862</v>
+        <v>0.38982365765561222</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.68214998653702974</v>
+        <v>7.9825795779816078E-2</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.146361385189784</v>
+        <v>0.5903503453312724</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.104151584958426</v>
+        <v>8.1819035020719522E-2</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19228582468295019</v>
+        <v>0.8650874034618965</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.60732461751171107</v>
+        <v>0.19971837851580299</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11114960326075018</v>
+        <v>-0.13525079734620959</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60865333547550637</v>
+        <v>0.40287287270207162</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.19461181521475157</v>
+        <v>0.19677937318000627</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43189157551394719</v>
+        <v>0.75853033685767079</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0030011369143419</v>
+        <v>0.55901579517651157</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.8676498218413835E-2</v>
+        <v>6.537048926124811E-2</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50191268269250511</v>
+        <v>1.2613008294686598</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1796651994982228</v>
+        <v>0.91402005126736841</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14200460540124049</v>
+        <v>0.2483726174615033</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92310336121174452</v>
+        <v>0.92847989640701378</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26968005762356095</v>
+        <v>1.2957677259393734</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24635659577406077</v>
+        <v>0.49380246781187598</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81123485277251617</v>
+        <v>-0.20858083104302194</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.44961317374297249</v>
+        <v>-0.54399830866754706</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44510406810884318</v>
+        <v>-0.38761439742773929</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24891983751085434</v>
+        <v>0.6191848944655991</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.56770566068538475</v>
+        <v>-0.19427824621078038</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33856939781674789</v>
+        <v>-0.39482109167740842</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91717319758625626</v>
+        <v>0.8673567245250231</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.66017322651211408</v>
+        <v>1.1124440481292095</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10341368298742082</v>
+        <v>-0.61583022997541681</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11525904000877296</v>
+        <v>1.098959703253765</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79935938109283322</v>
+        <v>-2.9524163773823942E-2</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.44018697787532957</v>
+        <v>-0.3600799838611155</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2406285525885603</v>
+        <v>-0.64228560420713809</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34824861472457136</v>
+        <v>1.240300204177633</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.49123216307431972</v>
+        <v>-1.3988771557791546E-2</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11177708387396135</v>
+        <v>0.23333923902120968</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0180507627195043</v>
+        <v>0.77605508585480165</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.40343929839472104</v>
+        <v>0.58619826890358517</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1759498633260508</v>
+        <v>0.11487906878679466</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.39516849717271119</v>
+        <v>2.4017922320512142E-2</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.42409549521195533</v>
+        <v>0.15259204176740715</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.15322047305401432</v>
+        <v>-0.58749038324708946</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96127738004601926</v>
+        <v>1.0404613241778622</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8646232883624556E-2</v>
+        <v>0.25886136682117122</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28484883879434131</v>
+        <v>1.0300066825570873</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.55360946279062584</v>
+        <v>1.1456078114509864</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73921198928478593</v>
+        <v>-1.3196555973761681E-2</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14782572290044005</v>
+        <v>0.96503390763277386</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21439280338699285</v>
+        <v>0.54032217484477685</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32362383786988924</v>
+        <v>0.60850475770395795</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.348617233902786E-2</v>
+        <v>0.98566531321203366</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24782893369227654</v>
+        <v>-0.18462949547490393</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45412963821204655</v>
+        <v>-0.14294439153880334</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.50483656586079251</v>
+        <v>-0.31150737480235002</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54091707755365892</v>
+        <v>-0.68124330321990634</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2572508298207719</v>
+        <v>0.25771808806834406</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6920899090831274</v>
+        <v>-0.25119926521753277</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38444613935382477</v>
+        <v>0.69487974757780946</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67584742257927921</v>
+        <v>-0.19241093133489895</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37757772708052828</v>
+        <v>-0.14093165797279772</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.5082090591256283</v>
+        <v>0.73187720569271808</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16210195740301936</v>
+        <v>-0.42449654800442471</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37166608179910909</v>
+        <v>0.18672429930792678</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97347459051731722</v>
+        <v>1.0607135531087484</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99840742198488086</v>
+        <v>-0.53831359986420368</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51658514107935738</v>
+        <v>0.67189503003287276</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1193245033519572</v>
+        <v>0.42224734244090967</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2722931334637493</v>
+        <v>0.14115784783612861</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9944692883068138</v>
+        <v>0.12451250631284339</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.26093759205677536</v>
+        <v>1.1237580783527503</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16600818500301839</v>
+        <v>0.50170203923111645</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40662398249580201</v>
+        <v>0.46935539220470512</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2038000717795849</v>
+        <v>-0.1795947647437901</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2105672928895399</v>
+        <v>0.42174765335448394</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91467187412658779</v>
+        <v>-0.13777928502522729</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8000424146945424</v>
+        <v>1.1319861056487095</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67930124488308685</v>
+        <v>0.97451303817837176</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37155354703148036</v>
+        <v>-3.8882765681267362E-2</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0909192157075023</v>
+        <v>1.1561369981361773</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59144445680366897</v>
+        <v>0.47731602303027287</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.60700002470571102</v>
+        <v>0.20346844205808967</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64625421176154352</v>
+        <v>0.46504798869982311</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.44891612016975202</v>
+        <v>-0.10625878747168493</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.46694647280448764</v>
+        <v>1.1099203530435169</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58059995570902556</v>
+        <v>0.92455369296543388</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46032067831672197</v>
+        <v>0.48065106542311731</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0322745153896089</v>
+        <v>1.0908921610528881</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2480382415773172</v>
+        <v>0.84764641297751275</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.69570418703283199</v>
+        <v>0.80835857959668411</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28111185597412613</v>
+        <v>0.8403995568474949</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.61259515292424682</v>
+        <v>0.30002422688376162</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.55338117764826733</v>
+        <v>-0.62799041758680008</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2342093037906388</v>
+        <v>-0.22615141160530694</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1086994021613468</v>
+        <v>0.79562428512359484</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32777111835107764</v>
+        <v>-0.61948711241904131</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22471511280699907</v>
+        <v>-0.60647804270407213</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17361726671137001</v>
+        <v>-0.57773794145771995</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.56584020193857043</v>
+        <v>0.86119814570905029</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24955286019041778</v>
+        <v>-0.13764336155895207</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54333984056727846</v>
+        <v>0.93324479959088125</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.293302356804324</v>
+        <v>-0.43864330593105572</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18890505878306096</v>
+        <v>8.8811621994588918E-5</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84806012347247495</v>
+        <v>0.55650751401960252</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96475404418042632</v>
+        <v>0.80820445777595573</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1627874298707521E-2</v>
+        <v>0.70100339165873948</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55547241095959365</v>
+        <v>-0.64095400810448533</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82303824960514005</v>
+        <v>-0.30274464293314973</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5885296688252577E-2</v>
+        <v>-4.6020864992482924E-2</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.39806249614092781</v>
+        <v>-0.16778148268228277</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90058753750591691</v>
+        <v>0.9799960427515042</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30476699144189512</v>
+        <v>-0.57397847183778361</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7888264852286939E-2</v>
+        <v>0.35774414203329163</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53322663827855066</v>
+        <v>-0.47547681529813879</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.59721165153962974</v>
+        <v>-0.55461721173628309</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74621297920225094</v>
+        <v>0.24926497849639229</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.7056150277823088E-2</v>
+        <v>-0.68884939107887777</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2489268980807335</v>
+        <v>0.31697873071034</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29347792360712122</v>
+        <v>0.75011253033297032</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.10953480987086506</v>
+        <v>-0.31465495494666329</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50413908395187557</v>
+        <v>1.2989287766507935</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30258923773964619</v>
+        <v>-1.5953187253874956E-2</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0069194678502964</v>
+        <v>0.35084245957437288</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.33358817868493484</v>
+        <v>0.43387233860742502</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3173360113210022</v>
+        <v>0.62380213509284022</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24813239543217325</v>
+        <v>0.85616178187605319</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46960308845926124</v>
+        <v>0.70530348190623493</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1702577939565597</v>
+        <v>-0.23304074656887708</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.9282921525648975E-2</v>
+        <v>0.2441387447522152</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.21404883263574748</v>
+        <v>1.277969406265111</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1287706788755258</v>
+        <v>0.78944526830408401</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.5564617228322852E-2</v>
+        <v>0.26346295984002532</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5745781542185231</v>
+        <v>-0.4870393000808344</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.43555264263850324</v>
+        <v>1.1429336340287026</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48573629860893863</v>
+        <v>0.63851144651014891</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.44234733693621653</v>
+        <v>0.98702467158433604</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25884622485644115</v>
+        <v>-0.31860014888847576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>